<commit_message>
inst/example_data_basic/emeScheme.xlsx: Update version definition
</commit_message>
<xml_diff>
--- a/inst/example_data/basic/emeScheme.xlsx
+++ b/inst/example_data/basic/emeScheme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainer/Documents/Projects/DataManagementAndStrategy/emeScheme/inst/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainerkrug/git/emeScheme/inst/example_data/basic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485B5043-89DA-5445-B174-79354C0E5257}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30D359C-4846-BC48-AA53-7786EE5CFB42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOCUMENTATION" sheetId="1" r:id="rId1"/>
@@ -1313,7 +1313,7 @@
     <t>presens Optode, microscopy</t>
   </si>
   <si>
-    <t>DATA_v0.9.5</t>
+    <t>DATA emeScheme v0.9.5</t>
   </si>
 </sst>
 </file>

</xml_diff>